<commit_message>
Added data for manitoba
</commit_message>
<xml_diff>
--- a/app/files/manitoba draft final 1 march 2018.xlsx
+++ b/app/files/manitoba draft final 1 march 2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -912,7 +912,7 @@
         <xdr:cNvPr id="2" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{46576D53-87EE-4C40-A5BD-E72E522FE095}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46576D53-87EE-4C40-A5BD-E72E522FE095}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -960,7 +960,7 @@
         <xdr:cNvPr id="3" name="AutoShape 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{443D3815-EF55-4B69-B57A-737B2ACE9071}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{443D3815-EF55-4B69-B57A-737B2ACE9071}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1008,7 +1008,7 @@
         <xdr:cNvPr id="4" name="AutoShape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3043A740-FCE5-412B-9B05-860218FC39CD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3043A740-FCE5-412B-9B05-860218FC39CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1056,7 +1056,7 @@
         <xdr:cNvPr id="7" name="Rectangle 6" descr="http://umanitoba.ca/student/admissions/programs/">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C99D51AB-59CB-4DBB-B56B-936C3ED44F0E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C99D51AB-59CB-4DBB-B56B-936C3ED44F0E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1376,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="K38" zoomScale="108" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>